<commit_message>
Proyecciones con rojos redux
</commit_message>
<xml_diff>
--- a/output/proyecciones/proyeccion_pea_por_sexo.xlsx
+++ b/output/proyecciones/proyeccion_pea_por_sexo.xlsx
@@ -489,13 +489,13 @@
         <v>45658</v>
       </c>
       <c r="B9">
-        <v>990108.381467861</v>
+        <v>990111.3636582257</v>
       </c>
       <c r="C9">
-        <v>831308.8434214069</v>
+        <v>831314.4975979078</v>
       </c>
       <c r="D9">
-        <v>1821417.224889268</v>
+        <v>1821425.861256134</v>
       </c>
     </row>
     <row r="10">
@@ -503,13 +503,13 @@
         <v>47484</v>
       </c>
       <c r="B10">
-        <v>1009820.519324138</v>
+        <v>1009838.458882504</v>
       </c>
       <c r="C10">
-        <v>850338.6010015674</v>
+        <v>850373.6581766765</v>
       </c>
       <c r="D10">
-        <v>1860159.120325706</v>
+        <v>1860212.117059181</v>
       </c>
     </row>
     <row r="11">
@@ -517,13 +517,13 @@
         <v>49310</v>
       </c>
       <c r="B11">
-        <v>1027478.16762167</v>
+        <v>1027531.694762051</v>
       </c>
       <c r="C11">
-        <v>868049.6442138629</v>
+        <v>868156.3520049311</v>
       </c>
       <c r="D11">
-        <v>1895527.811835533</v>
+        <v>1895688.046766982</v>
       </c>
     </row>
     <row r="12">
@@ -531,13 +531,13 @@
         <v>51136</v>
       </c>
       <c r="B12">
-        <v>1038255.800326183</v>
+        <v>1038369.02837113</v>
       </c>
       <c r="C12">
-        <v>878324.5771338706</v>
+        <v>878556.1803677904</v>
       </c>
       <c r="D12">
-        <v>1916580.377460054</v>
+        <v>1916925.20873892</v>
       </c>
     </row>
     <row r="13">
@@ -545,13 +545,13 @@
         <v>52963</v>
       </c>
       <c r="B13">
-        <v>1037450.526776197</v>
+        <v>1037644.072918339</v>
       </c>
       <c r="C13">
-        <v>879885.7741500348</v>
+        <v>880302.1978995795</v>
       </c>
       <c r="D13">
-        <v>1917336.300926232</v>
+        <v>1917946.270817919</v>
       </c>
     </row>
     <row r="14">
@@ -559,13 +559,13 @@
         <v>54789</v>
       </c>
       <c r="B14">
-        <v>1030921.231681681</v>
+        <v>1031218.814306257</v>
       </c>
       <c r="C14">
-        <v>876767.7485826823</v>
+        <v>877441.7585444573</v>
       </c>
       <c r="D14">
-        <v>1907688.980264363</v>
+        <v>1908660.572850714</v>
       </c>
     </row>
     <row r="15">
@@ -573,13 +573,13 @@
         <v>56615</v>
       </c>
       <c r="B15">
-        <v>1018536.002568605</v>
+        <v>1018946.673769818</v>
       </c>
       <c r="C15">
-        <v>865345.1590901307</v>
+        <v>866333.4608667413</v>
       </c>
       <c r="D15">
-        <v>1883881.161658735</v>
+        <v>1885280.134636559</v>
       </c>
     </row>
     <row r="16">
@@ -587,13 +587,13 @@
         <v>58441</v>
       </c>
       <c r="B16">
-        <v>999013.8374270187</v>
+        <v>999525.3877778889</v>
       </c>
       <c r="C16">
-        <v>844661.3526439342</v>
+        <v>846011.7320133122</v>
       </c>
       <c r="D16">
-        <v>1843675.190070953</v>
+        <v>1845537.119791201</v>
       </c>
     </row>
     <row r="17">
@@ -601,13 +601,13 @@
         <v>60268</v>
       </c>
       <c r="B17">
-        <v>972186.0112812264</v>
+        <v>972793.8281127313</v>
       </c>
       <c r="C17">
-        <v>819894.6328608491</v>
+        <v>821655.2534553671</v>
       </c>
       <c r="D17">
-        <v>1792080.644142075</v>
+        <v>1794449.081568098</v>
       </c>
     </row>
     <row r="18">
@@ -615,13 +615,13 @@
         <v>62094</v>
       </c>
       <c r="B18">
-        <v>943208.7152605215</v>
+        <v>943897.9557722975</v>
       </c>
       <c r="C18">
-        <v>792941.4393109806</v>
+        <v>795191.0654827683</v>
       </c>
       <c r="D18">
-        <v>1736150.154571502</v>
+        <v>1739089.021255066</v>
       </c>
     </row>
     <row r="19">
@@ -629,13 +629,13 @@
         <v>63920</v>
       </c>
       <c r="B19">
-        <v>908414.0898790854</v>
+        <v>909182.543202111</v>
       </c>
       <c r="C19">
-        <v>764206.258038302</v>
+        <v>766968.9717814658</v>
       </c>
       <c r="D19">
-        <v>1672620.347917387</v>
+        <v>1676151.514983577</v>
       </c>
     </row>
     <row r="20">
@@ -643,13 +643,13 @@
         <v>65746</v>
       </c>
       <c r="B20">
-        <v>863980.9891752839</v>
+        <v>864782.6833214258</v>
       </c>
       <c r="C20">
-        <v>724944.5790838501</v>
+        <v>728187.7033590564</v>
       </c>
       <c r="D20">
-        <v>1588925.568259134</v>
+        <v>1592970.386680482</v>
       </c>
     </row>
     <row r="21">
@@ -657,13 +657,13 @@
         <v>67573</v>
       </c>
       <c r="B21">
-        <v>814023.922221331</v>
+        <v>814816.909249138</v>
       </c>
       <c r="C21">
-        <v>682481.1110278579</v>
+        <v>686234.4709944156</v>
       </c>
       <c r="D21">
-        <v>1496505.033249189</v>
+        <v>1501051.380243554</v>
       </c>
     </row>
     <row r="22">
@@ -671,13 +671,13 @@
         <v>69399</v>
       </c>
       <c r="B22">
-        <v>763094.0345235339</v>
+        <v>763954.3121890175</v>
       </c>
       <c r="C22">
-        <v>639506.4296585751</v>
+        <v>643899.7470905373</v>
       </c>
       <c r="D22">
-        <v>1402600.464182109</v>
+        <v>1407854.059279555</v>
       </c>
     </row>
     <row r="23">
@@ -685,13 +685,13 @@
         <v>71225</v>
       </c>
       <c r="B23">
-        <v>707408.8827886988</v>
+        <v>708329.7785302646</v>
       </c>
       <c r="C23">
-        <v>590740.9778599025</v>
+        <v>595847.0536259327</v>
       </c>
       <c r="D23">
-        <v>1298149.860648601</v>
+        <v>1304176.832156197</v>
       </c>
     </row>
     <row r="24">
@@ -699,13 +699,13 @@
         <v>73051</v>
       </c>
       <c r="B24">
-        <v>647598.4055939707</v>
+        <v>648565.7703387433</v>
       </c>
       <c r="C24">
-        <v>539673.8945054142</v>
+        <v>545519.484876293</v>
       </c>
       <c r="D24">
-        <v>1187272.300099385</v>
+        <v>1194085.255215036</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tasas modelo solo mujeres
</commit_message>
<xml_diff>
--- a/output/proyecciones/proyeccion_pea_por_sexo.xlsx
+++ b/output/proyecciones/proyeccion_pea_por_sexo.xlsx
@@ -489,13 +489,13 @@
         <v>45658</v>
       </c>
       <c r="B9">
-        <v>990111</v>
+        <v>986696</v>
       </c>
       <c r="C9">
-        <v>831314</v>
+        <v>820146</v>
       </c>
       <c r="D9">
-        <v>1821425</v>
+        <v>1806842</v>
       </c>
     </row>
     <row r="10">
@@ -503,13 +503,13 @@
         <v>47484</v>
       </c>
       <c r="B10">
-        <v>1009838</v>
+        <v>1001979</v>
       </c>
       <c r="C10">
-        <v>850374</v>
+        <v>827473</v>
       </c>
       <c r="D10">
-        <v>1860212</v>
+        <v>1829452</v>
       </c>
     </row>
     <row r="11">
@@ -517,13 +517,13 @@
         <v>49310</v>
       </c>
       <c r="B11">
-        <v>1027532</v>
+        <v>1014497</v>
       </c>
       <c r="C11">
-        <v>868156</v>
+        <v>833234</v>
       </c>
       <c r="D11">
-        <v>1895688</v>
+        <v>1847731</v>
       </c>
     </row>
     <row r="12">
@@ -531,13 +531,13 @@
         <v>51136</v>
       </c>
       <c r="B12">
-        <v>1038369</v>
+        <v>1018142</v>
       </c>
       <c r="C12">
-        <v>878556</v>
+        <v>832331</v>
       </c>
       <c r="D12">
-        <v>1916925</v>
+        <v>1850473</v>
       </c>
     </row>
     <row r="13">
@@ -545,13 +545,13 @@
         <v>52963</v>
       </c>
       <c r="B13">
-        <v>1037644</v>
+        <v>1010742</v>
       </c>
       <c r="C13">
-        <v>880302</v>
+        <v>823371</v>
       </c>
       <c r="D13">
-        <v>1917946</v>
+        <v>1834113</v>
       </c>
     </row>
     <row r="14">
@@ -559,13 +559,13 @@
         <v>54789</v>
       </c>
       <c r="B14">
-        <v>1031219</v>
+        <v>998867</v>
       </c>
       <c r="C14">
-        <v>877442</v>
+        <v>811318</v>
       </c>
       <c r="D14">
-        <v>1908661</v>
+        <v>1810185</v>
       </c>
     </row>
     <row r="15">
@@ -573,13 +573,13 @@
         <v>56615</v>
       </c>
       <c r="B15">
-        <v>1018947</v>
+        <v>981215</v>
       </c>
       <c r="C15">
-        <v>866333</v>
+        <v>794034</v>
       </c>
       <c r="D15">
-        <v>1885280</v>
+        <v>1775249</v>
       </c>
     </row>
     <row r="16">
@@ -587,13 +587,13 @@
         <v>58441</v>
       </c>
       <c r="B16">
-        <v>999525</v>
+        <v>957784</v>
       </c>
       <c r="C16">
-        <v>846012</v>
+        <v>771008</v>
       </c>
       <c r="D16">
-        <v>1845537</v>
+        <v>1728792</v>
       </c>
     </row>
     <row r="17">
@@ -601,13 +601,13 @@
         <v>60268</v>
       </c>
       <c r="B17">
-        <v>972794</v>
+        <v>930776</v>
       </c>
       <c r="C17">
-        <v>821655</v>
+        <v>747323</v>
       </c>
       <c r="D17">
-        <v>1794449</v>
+        <v>1678099</v>
       </c>
     </row>
     <row r="18">
@@ -615,13 +615,13 @@
         <v>62094</v>
       </c>
       <c r="B18">
-        <v>943898</v>
+        <v>905315</v>
       </c>
       <c r="C18">
-        <v>795191</v>
+        <v>724604</v>
       </c>
       <c r="D18">
-        <v>1739089</v>
+        <v>1629919</v>
       </c>
     </row>
     <row r="19">
@@ -629,13 +629,13 @@
         <v>63920</v>
       </c>
       <c r="B19">
-        <v>909183</v>
+        <v>877840</v>
       </c>
       <c r="C19">
-        <v>766969</v>
+        <v>703490</v>
       </c>
       <c r="D19">
-        <v>1676152</v>
+        <v>1581330</v>
       </c>
     </row>
     <row r="20">
@@ -643,13 +643,13 @@
         <v>65746</v>
       </c>
       <c r="B20">
-        <v>864783</v>
+        <v>844957</v>
       </c>
       <c r="C20">
-        <v>728188</v>
+        <v>677689</v>
       </c>
       <c r="D20">
-        <v>1592971</v>
+        <v>1522646</v>
       </c>
     </row>
     <row r="21">
@@ -657,13 +657,13 @@
         <v>67573</v>
       </c>
       <c r="B21">
-        <v>814817</v>
+        <v>811724</v>
       </c>
       <c r="C21">
-        <v>686234</v>
+        <v>651264</v>
       </c>
       <c r="D21">
-        <v>1501051</v>
+        <v>1462988</v>
       </c>
     </row>
     <row r="22">
@@ -671,13 +671,13 @@
         <v>69399</v>
       </c>
       <c r="B22">
-        <v>763954</v>
+        <v>781636</v>
       </c>
       <c r="C22">
-        <v>643900</v>
+        <v>628960</v>
       </c>
       <c r="D22">
-        <v>1407854</v>
+        <v>1410596</v>
       </c>
     </row>
     <row r="23">
@@ -685,13 +685,13 @@
         <v>71225</v>
       </c>
       <c r="B23">
-        <v>708330</v>
+        <v>750691</v>
       </c>
       <c r="C23">
-        <v>595847</v>
+        <v>605088</v>
       </c>
       <c r="D23">
-        <v>1304177</v>
+        <v>1355779</v>
       </c>
     </row>
     <row r="24">
@@ -699,13 +699,13 @@
         <v>73051</v>
       </c>
       <c r="B24">
-        <v>648566</v>
+        <v>719497</v>
       </c>
       <c r="C24">
-        <v>545519</v>
+        <v>582464</v>
       </c>
       <c r="D24">
-        <v>1194085</v>
+        <v>1301961</v>
       </c>
     </row>
   </sheetData>

</xml_diff>